<commit_message>
Updated CHE model - 2025-07-31 16:29
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0831819F-3D23-44E2-8E89-8F0076D5210C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90B6718-3D2A-4EA3-B736-93C797651EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,TaD,Wb0122h12,Wb0121h14,Wb0121h16,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h12,Tc0917h08,Tc0917h17</t>
-  </si>
-  <si>
-    <t>SaP,Tc0916h06,Tc0917h01,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,RaN,Tc0917h20,Wb0122h20,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Wb0121h05,Wb0121h24,Tc0917h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02</t>
+    <t>Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12,TaD,Wb0122h12,Wb0121h13,Tc0916h10,Tc0917h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h14,Wb0121h16,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</t>
+  </si>
+  <si>
+    <t>TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24,RaN,Tc0917h20,Wb0122h20,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaN,Tc0916h03,Tc0916h23,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h04</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>SaP,Tc0916h06,Tc0917h01,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,RaN,Tc0917h20,Wb0122h20,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Wb0121h05,Wb0121h24,Tc0917h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02</v>
+        <v>TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24,RaN,Tc0917h20,Wb0122h20,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaN,Tc0916h03,Tc0916h23,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h04</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,TaD,Wb0122h12,Wb0121h14,Wb0121h16,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h12,Tc0917h08,Tc0917h17</v>
+        <v>Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12,TaD,Wb0122h12,Wb0121h13,Tc0916h10,Tc0917h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h14,Wb0121h16,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31BBFF8-2168-4934-A124-F3C028152A01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47759AEE-0024-41AC-B2A8-287B48C04E2D}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6687EA0-7CD9-4D92-89CF-7209B2AEFD6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDFB1CB-D576-4B3F-8668-51F2A50A27E9}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3079,7 +3079,7 @@
         <v>33</v>
       </c>
       <c r="N4">
-        <v>0.27553730672996718</v>
+        <v>0.27553730672996724</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="N5">
-        <v>0.39690767947648675</v>
+        <v>0.2560595367934817</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3181,10 +3181,10 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="N7">
-        <v>0.2560595367934817</v>
+        <v>0.39690767947648675</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59321E63-7EFF-4092-8A12-1648CA0E66A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B858B1-4D04-473D-8F76-471CB3B07162}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-07-31 19:00
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90B6718-3D2A-4EA3-B736-93C797651EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B60E172-5EE9-452C-9653-C81B2E609B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12,TaD,Wb0122h12,Wb0121h13,Tc0916h10,Tc0917h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h14,Wb0121h16,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</t>
-  </si>
-  <si>
-    <t>TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24,RaN,Tc0917h20,Wb0122h20,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaN,Tc0916h03,Tc0916h23,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h04</t>
+    <t>Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0917h08,Tc0917h17,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h10,Tc0917h14,TaD,Wb0122h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12</t>
+  </si>
+  <si>
+    <t>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaN,Tc0917h20,Wb0122h20,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24,RaN,Tc0917h20,Wb0122h20,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaN,Tc0916h03,Tc0916h23,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h04</v>
+        <v>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaN,Tc0917h20,Wb0122h20,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12,TaD,Wb0122h12,Wb0121h13,Tc0916h10,Tc0917h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h14,Wb0121h16,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14</v>
+        <v>Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0917h08,Tc0917h17,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h10,Tc0917h14,TaD,Wb0122h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47759AEE-0024-41AC-B2A8-287B48C04E2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BA5E4D-7801-4532-BF1F-93C08FF3057F}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDFB1CB-D576-4B3F-8668-51F2A50A27E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2DD1E-55FC-43EE-8809-26D2EECF31B4}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>0.2560595367934817</v>
+        <v>0.27149547700006416</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N6">
-        <v>0.27149547700006416</v>
+        <v>0.2560595367934817</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B858B1-4D04-473D-8F76-471CB3B07162}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E96084-047B-48AF-881B-732F4D82CED9}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-07-31 23:25
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B60E172-5EE9-452C-9653-C81B2E609B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A76C6E-7BBB-4804-A35F-93568EF61D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0917h08,Tc0917h17,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h10,Tc0917h14,TaD,Wb0122h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12</t>
-  </si>
-  <si>
-    <t>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaN,Tc0917h20,Wb0122h20,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24</t>
+    <t>TaD,Wb0122h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0916h11,Wb0121h09,Wb0121h13,Tc0917h08,Tc0917h17,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h10,Tc0917h14,Tc0916h12,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h18,Wb0121h08,Wb0121h18,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h14,Wb0121h16</t>
+  </si>
+  <si>
+    <t>RaN,Tc0917h20,Wb0122h20,TaN,Tc0916h03,Tc0916h23,TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0917h24,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaP,Tc0916h06,Tc0917h01,Wb0121h05,Wb0121h24,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h02,Tc0917h06,WaP,Wb0122h22</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,SaP,Tc0916h06,Tc0917h01,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaN,Tc0917h20,Wb0122h20,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24</v>
+        <v>RaN,Tc0917h20,Wb0122h20,TaN,Tc0916h03,Tc0916h23,TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0917h24,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaP,Tc0916h06,Tc0917h01,Wb0121h05,Wb0121h24,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0916h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h02,Tc0917h06,WaP,Wb0122h22</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0917h08,Tc0917h17,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h10,Tc0917h14,TaD,Wb0122h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12</v>
+        <v>TaD,Wb0122h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0916h11,Wb0121h09,Wb0121h13,Tc0917h08,Tc0917h17,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h10,Tc0917h14,Tc0916h12,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0917h18,Wb0121h08,Wb0121h18,RaD,Wb0122h11,Wb0122h15,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h14,Wb0121h16</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BA5E4D-7801-4532-BF1F-93C08FF3057F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB253621-2A00-426C-9C8D-49EC3EBB31C7}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E2DD1E-55FC-43EE-8809-26D2EECF31B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C674F2-EE52-473C-8398-3AEC680D2CF7}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N5">
-        <v>0.27149547700006416</v>
+        <v>0.39690767947648675</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3181,10 +3181,10 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N7">
-        <v>0.39690767947648675</v>
+        <v>0.27149547700006416</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E96084-047B-48AF-881B-732F4D82CED9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F7D67A-0249-4D5C-9A11-694EE6509604}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-01 02:36
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_CHE/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EA4D1E-EB80-4A0A-B3EC-FD6D5F9E61D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A5C8B9-2BE8-41F0-A6E0-7AC1C507F0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="302">
   <si>
     <t>UC_N</t>
   </si>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0917h08,Tc0917h17,TaD,Wb0122h12,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0916h10,Tc0917h14,RaD,Wb0122h11,Wb0122h15,Tc0916h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13</t>
-  </si>
-  <si>
-    <t>Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,RaN,Tc0917h20,Wb0122h20,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0917h24,TaN,Tc0916h03,Tc0916h23,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h23,Wb0121h02,Wb0121h06</t>
+    <t>SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,TaD,Wb0122h12,Tc0916h12,Wb0121h14,Wb0121h16</t>
+  </si>
+  <si>
+    <t>SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h24,Tc0917h05,Tc0917h19,Wb0121h05,Wb0121h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h23,Wb0121h02,Wb0121h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,RaN,Tc0917h20,Wb0122h20,Tc0917h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>Tc0916h04,SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,RaN,Tc0917h20,Wb0122h20,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Wb0121h05,Wb0121h24,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0917h24,TaN,Tc0916h03,Tc0916h23,Tc0916h24,Tc0917h05,Tc0917h19,Tc0917h23,Wb0121h02,Wb0121h06</v>
+        <v>SaP,Tc0916h06,Tc0917h01,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0916h04,TaN,Tc0916h03,Tc0916h23,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h24,Tc0917h05,Tc0917h19,Wb0121h05,Wb0121h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h23,Wb0121h02,Wb0121h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,RaN,Tc0917h20,Wb0122h20,Tc0917h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0917h08,Tc0917h17,TaD,Wb0122h12,Tc0916h11,Wb0121h09,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Wb0121h14,Wb0121h16,Wb0121h13,Tc0916h10,Tc0917h14,RaD,Wb0122h11,Wb0122h15,Tc0916h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13</v>
+        <v>SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h11,Wb0121h09,Tc0917h08,Tc0917h17,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,TaD,Wb0122h12,Tc0916h12,Wb0121h14,Wb0121h16</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B86AAE9-CC9E-46C8-97BC-7B39B8C51936}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF94AE2-456A-4B3E-BB7D-A7A201630CB0}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA522E50-E3A8-4CBA-8BA3-543733782EF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023F9186-0F2A-42BD-96D9-7851D15001A0}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3079,7 +3079,7 @@
         <v>33</v>
       </c>
       <c r="N4">
-        <v>0.27553730672996729</v>
+        <v>0.27553730672996718</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>0.39690767947648681</v>
+        <v>0.27149547700006416</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3149,7 +3149,7 @@
         <v>22</v>
       </c>
       <c r="N6">
-        <v>0.25605953679348176</v>
+        <v>0.2560595367934817</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -3181,10 +3181,10 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N7">
-        <v>0.27149547700006416</v>
+        <v>0.39690767947648675</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,8 +5900,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3726F32-567F-4264-9EB8-D4C26A7660DE}">
-  <dimension ref="B2:O211"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E1D975-1328-43C6-B2AF-87907EA299AC}">
+  <dimension ref="B2:O219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5970,7 +5970,7 @@
         <v>178</v>
       </c>
       <c r="J4">
-        <v>0.15571510693448795</v>
+        <v>0.14930583190901445</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -5979,7 +5979,7 @@
         <v>178</v>
       </c>
       <c r="O4">
-        <v>0.14282545429258064</v>
+        <v>0.14944926001652092</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.45">
@@ -6002,7 +6002,7 @@
         <v>181</v>
       </c>
       <c r="J5">
-        <v>7.3994799682947143E-2</v>
+        <v>7.9887830153514902E-2</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
@@ -6011,7 +6011,7 @@
         <v>181</v>
       </c>
       <c r="O5">
-        <v>0.25624015491544871</v>
+        <v>0.21001703682311934</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
@@ -6034,7 +6034,7 @@
         <v>182</v>
       </c>
       <c r="J6">
-        <v>2.2228394189831344E-2</v>
+        <v>2.2643791796899834E-2</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
@@ -6043,7 +6043,7 @@
         <v>182</v>
       </c>
       <c r="O6">
-        <v>0.16082919843655996</v>
+        <v>0.15503284403944284</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.45">
@@ -6066,7 +6066,7 @@
         <v>183</v>
       </c>
       <c r="J7">
-        <v>0.13750571422592917</v>
+        <v>0.13136922162635617</v>
       </c>
       <c r="M7" t="s">
         <v>14</v>
@@ -6075,7 +6075,7 @@
         <v>183</v>
       </c>
       <c r="O7">
-        <v>0.12984476109861576</v>
+        <v>0.13897262709351366</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.45">
@@ -6098,7 +6098,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>6.3873294052778223E-2</v>
+        <v>6.9671322655511764E-2</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
@@ -6107,7 +6107,7 @@
         <v>184</v>
       </c>
       <c r="O8">
-        <v>0.15755866008140496</v>
+        <v>0.17798010888368254</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.45">
@@ -6130,7 +6130,7 @@
         <v>185</v>
       </c>
       <c r="J9">
-        <v>1.9476837797143196E-2</v>
+        <v>1.9512746381401977E-2</v>
       </c>
       <c r="M9" t="s">
         <v>14</v>
@@ -6139,7 +6139,7 @@
         <v>185</v>
       </c>
       <c r="O9">
-        <v>0.10323610634869729</v>
+        <v>9.394838899141722E-2</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.45">
@@ -6162,7 +6162,7 @@
         <v>186</v>
       </c>
       <c r="J10">
-        <v>0.14459613078253578</v>
+        <v>0.13804823887601783</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
@@ -6171,7 +6171,7 @@
         <v>186</v>
       </c>
       <c r="O10">
-        <v>0.17607029986549216</v>
+        <v>0.18640735087813476</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.45">
@@ -6194,7 +6194,7 @@
         <v>187</v>
       </c>
       <c r="J11">
-        <v>6.762675210559474E-2</v>
+        <v>7.3721834441919695E-2</v>
       </c>
       <c r="M11" t="s">
         <v>14</v>
@@ -6203,7 +6203,7 @@
         <v>187</v>
       </c>
       <c r="O11">
-        <v>0.25154265032329604</v>
+        <v>0.24501192769235791</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.45">
@@ -6226,7 +6226,7 @@
         <v>188</v>
       </c>
       <c r="J12">
-        <v>2.0954164162503397E-2</v>
+        <v>2.1229176882329899E-2</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -6235,7 +6235,7 @@
         <v>188</v>
       </c>
       <c r="O12">
-        <v>0.18113574103502494</v>
+        <v>0.18028117146072575</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.45">
@@ -6258,7 +6258,7 @@
         <v>189</v>
       </c>
       <c r="J13">
-        <v>8.0385842442850543E-5</v>
+        <v>7.8403959861603572E-5</v>
       </c>
       <c r="M13" t="s">
         <v>14</v>
@@ -6290,7 +6290,7 @@
         <v>190</v>
       </c>
       <c r="J14">
-        <v>8.0578265822871161E-5</v>
+        <v>7.7701303498394216E-5</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
@@ -6322,7 +6322,7 @@
         <v>191</v>
       </c>
       <c r="J15">
-        <v>8.4341211921052061E-5</v>
+        <v>7.7887300771008463E-5</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
@@ -6354,7 +6354,7 @@
         <v>192</v>
       </c>
       <c r="J16">
-        <v>9.2038147121876614E-5</v>
+        <v>8.1524580768798139E-5</v>
       </c>
       <c r="M16" t="s">
         <v>14</v>
@@ -6386,7 +6386,7 @@
         <v>193</v>
       </c>
       <c r="J17">
-        <v>1.0379735367869191E-4</v>
+        <v>8.8964471673367909E-5</v>
       </c>
       <c r="M17" t="s">
         <v>14</v>
@@ -6418,7 +6418,7 @@
         <v>194</v>
       </c>
       <c r="J18">
-        <v>1.1662557901339953E-4</v>
+        <v>1.0033097166646063E-4</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -6450,7 +6450,7 @@
         <v>195</v>
       </c>
       <c r="J19">
-        <v>1.26417791018893E-4</v>
+        <v>1.1273078984074359E-4</v>
       </c>
       <c r="M19" t="s">
         <v>14</v>
@@ -6482,7 +6482,7 @@
         <v>196</v>
       </c>
       <c r="J20">
-        <v>1.2941104359699143E-4</v>
+        <v>1.2219598438044626E-4</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -6514,7 +6514,7 @@
         <v>197</v>
       </c>
       <c r="J21">
-        <v>1.2971036885480125E-4</v>
+        <v>1.2508927528777895E-4</v>
       </c>
       <c r="M21" t="s">
         <v>14</v>
@@ -6546,7 +6546,7 @@
         <v>198</v>
       </c>
       <c r="J22">
-        <v>1.2971036885480128E-4</v>
+        <v>1.2537860437851221E-4</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -6578,7 +6578,7 @@
         <v>199</v>
       </c>
       <c r="J23">
-        <v>1.2926138096808651E-4</v>
+        <v>1.2537860437851223E-4</v>
       </c>
       <c r="M23" t="s">
         <v>14</v>
@@ -6610,7 +6610,7 @@
         <v>200</v>
       </c>
       <c r="J24">
-        <v>1.2926138096808651E-4</v>
+        <v>1.2494461074241231E-4</v>
       </c>
       <c r="M24" t="s">
         <v>14</v>
@@ -6642,7 +6642,7 @@
         <v>201</v>
       </c>
       <c r="J25">
-        <v>1.2780751543015298E-4</v>
+        <v>1.2494461074241231E-4</v>
       </c>
       <c r="M25" t="s">
         <v>14</v>
@@ -6674,7 +6674,7 @@
         <v>202</v>
       </c>
       <c r="J26">
-        <v>1.2759371167457451E-4</v>
+        <v>1.2353929801599357E-4</v>
       </c>
       <c r="M26" t="s">
         <v>14</v>
@@ -6706,7 +6706,7 @@
         <v>203</v>
       </c>
       <c r="J27">
-        <v>1.2731576679232251E-4</v>
+        <v>1.2333263437975552E-4</v>
       </c>
       <c r="M27" t="s">
         <v>14</v>
@@ -6738,7 +6738,7 @@
         <v>204</v>
       </c>
       <c r="J28">
-        <v>1.2695230040783915E-4</v>
+        <v>1.2306397165264606E-4</v>
       </c>
       <c r="M28" t="s">
         <v>14</v>
@@ -6770,7 +6770,7 @@
         <v>205</v>
       </c>
       <c r="J29">
-        <v>1.2594742275662038E-4</v>
+        <v>1.2271264347104137E-4</v>
       </c>
       <c r="M29" t="s">
         <v>14</v>
@@ -6802,7 +6802,7 @@
         <v>206</v>
       </c>
       <c r="J30">
-        <v>1.2492116472984376E-4</v>
+        <v>1.2174132438072256E-4</v>
       </c>
       <c r="M30" t="s">
         <v>14</v>
@@ -6834,7 +6834,7 @@
         <v>207</v>
       </c>
       <c r="J31">
-        <v>1.2135064201168349E-4</v>
+        <v>1.2074933892677992E-4</v>
       </c>
       <c r="M31" t="s">
         <v>14</v>
@@ -6866,7 +6866,7 @@
         <v>208</v>
       </c>
       <c r="J32">
-        <v>1.0986938033712016E-4</v>
+        <v>1.1729805620160449E-4</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -6898,7 +6898,7 @@
         <v>209</v>
       </c>
       <c r="J33">
-        <v>1.0307042090972515E-4</v>
+        <v>1.0620021893562124E-4</v>
       </c>
       <c r="M33" t="s">
         <v>14</v>
@@ -6930,7 +6930,7 @@
         <v>210</v>
       </c>
       <c r="J34">
-        <v>9.4582411813260274E-5</v>
+        <v>9.9628315303251257E-5</v>
       </c>
       <c r="M34" t="s">
         <v>14</v>
@@ -6962,7 +6962,7 @@
         <v>211</v>
       </c>
       <c r="J35">
-        <v>8.6137163467911115E-5</v>
+        <v>9.1423768944600697E-5</v>
       </c>
       <c r="M35" t="s">
         <v>14</v>
@@ -6991,16 +6991,16 @@
         <v>295</v>
       </c>
       <c r="I36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J36">
-        <v>8.0022376058367146E-5</v>
+        <v>8.3260555313197741E-5</v>
       </c>
       <c r="M36" t="s">
         <v>14</v>
       </c>
       <c r="N36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -7023,16 +7023,16 @@
         <v>295</v>
       </c>
       <c r="I37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J37">
-        <v>8.0877591080680988E-5</v>
+        <v>7.7804635316513227E-5</v>
       </c>
       <c r="M37" t="s">
         <v>14</v>
       </c>
       <c r="N37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -7055,16 +7055,16 @@
         <v>295</v>
       </c>
       <c r="I38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J38">
-        <v>8.5217807318923715E-5</v>
+        <v>7.7349975316789524E-5</v>
       </c>
       <c r="M38" t="s">
         <v>14</v>
       </c>
       <c r="N38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -7087,16 +7087,16 @@
         <v>295</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J39">
-        <v>9.4112043550987669E-5</v>
+        <v>7.8176629861741721E-5</v>
       </c>
       <c r="M39" t="s">
         <v>14</v>
       </c>
       <c r="N39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -7119,16 +7119,16 @@
         <v>295</v>
       </c>
       <c r="I40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J40">
-        <v>1.0559330522555099E-4</v>
+        <v>8.2371901677374111E-5</v>
       </c>
       <c r="M40" t="s">
         <v>14</v>
       </c>
       <c r="N40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -7151,16 +7151,16 @@
         <v>295</v>
       </c>
       <c r="I41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J41">
-        <v>1.2028162323379119E-4</v>
+        <v>9.096910894487698E-5</v>
       </c>
       <c r="M41" t="s">
         <v>14</v>
       </c>
       <c r="N41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -7183,16 +7183,16 @@
         <v>295</v>
       </c>
       <c r="I42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J42">
-        <v>1.2975312960591696E-4</v>
+        <v>1.0206694621086026E-4</v>
       </c>
       <c r="M42" t="s">
         <v>14</v>
       </c>
       <c r="N42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -7215,16 +7215,16 @@
         <v>295</v>
       </c>
       <c r="I43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J43">
-        <v>1.3003107448816896E-4</v>
+        <v>1.1626473802041423E-4</v>
       </c>
       <c r="M43" t="s">
         <v>14</v>
       </c>
       <c r="N43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -7247,16 +7247,16 @@
         <v>295</v>
       </c>
       <c r="I44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J44">
-        <v>1.2949656509922281E-4</v>
+        <v>1.2541993710575984E-4</v>
       </c>
       <c r="M44" t="s">
         <v>14</v>
       </c>
       <c r="N44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -7279,16 +7279,16 @@
         <v>295</v>
       </c>
       <c r="I45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J45">
-        <v>1.293469024703179E-4</v>
+        <v>1.2568859983286929E-4</v>
       </c>
       <c r="M45" t="s">
         <v>14</v>
       </c>
       <c r="N45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -7311,16 +7311,16 @@
         <v>295</v>
       </c>
       <c r="I46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J46">
-        <v>1.2947518472366496E-4</v>
+        <v>1.2517194074227419E-4</v>
       </c>
       <c r="M46" t="s">
         <v>14</v>
       </c>
       <c r="N46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -7343,16 +7343,16 @@
         <v>295</v>
       </c>
       <c r="I47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J47">
-        <v>1.2964622772812772E-4</v>
+        <v>1.2502727619690754E-4</v>
       </c>
       <c r="M47" t="s">
         <v>14</v>
       </c>
       <c r="N47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -7375,16 +7375,16 @@
         <v>295</v>
       </c>
       <c r="I48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J48">
-        <v>1.2866273045246681E-4</v>
+        <v>1.2515127437865036E-4</v>
       </c>
       <c r="M48" t="s">
         <v>14</v>
       </c>
       <c r="N48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O48">
         <v>0</v>
@@ -7407,16 +7407,16 @@
         <v>295</v>
       </c>
       <c r="I49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J49">
-        <v>1.283847855702148E-4</v>
+        <v>1.253166052876408E-4</v>
       </c>
       <c r="M49" t="s">
         <v>14</v>
       </c>
       <c r="N49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -7439,16 +7439,16 @@
         <v>295</v>
       </c>
       <c r="I50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J50">
-        <v>1.2810684068796283E-4</v>
+        <v>1.2436595256094579E-4</v>
       </c>
       <c r="M50" t="s">
         <v>14</v>
       </c>
       <c r="N50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -7471,16 +7471,16 @@
         <v>295</v>
       </c>
       <c r="I51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J51">
-        <v>1.2774337430347945E-4</v>
+        <v>1.2409728983383631E-4</v>
       </c>
       <c r="M51" t="s">
         <v>14</v>
       </c>
       <c r="N51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -7503,16 +7503,16 @@
         <v>295</v>
       </c>
       <c r="I52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J52">
-        <v>1.2697368078339697E-4</v>
+        <v>1.2382862710672688E-4</v>
       </c>
       <c r="M52" t="s">
         <v>14</v>
       </c>
       <c r="N52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -7535,16 +7535,16 @@
         <v>295</v>
       </c>
       <c r="I53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J53">
-        <v>1.2571223862548406E-4</v>
+        <v>1.2347729892512216E-4</v>
       </c>
       <c r="M53" t="s">
         <v>14</v>
       </c>
       <c r="N53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -7567,16 +7567,16 @@
         <v>295</v>
       </c>
       <c r="I54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J54">
-        <v>1.2188515140062963E-4</v>
+        <v>1.227333098346652E-4</v>
       </c>
       <c r="M54" t="s">
         <v>14</v>
       </c>
       <c r="N54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -7599,16 +7599,16 @@
         <v>295</v>
       </c>
       <c r="I55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J55">
-        <v>1.1019008597048786E-4</v>
+        <v>1.2151399438086069E-4</v>
       </c>
       <c r="M55" t="s">
         <v>14</v>
       </c>
       <c r="N55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -7631,16 +7631,16 @@
         <v>295</v>
       </c>
       <c r="I56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J56">
-        <v>1.0398977705871251E-4</v>
+        <v>1.178147152921996E-4</v>
       </c>
       <c r="M56" t="s">
         <v>14</v>
       </c>
       <c r="N56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O56">
         <v>0</v>
@@ -7663,16 +7663,16 @@
         <v>295</v>
       </c>
       <c r="I57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J57">
-        <v>9.4411368808797522E-5</v>
+        <v>1.065102143899783E-4</v>
       </c>
       <c r="M57" t="s">
         <v>14</v>
       </c>
       <c r="N57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O57">
         <v>0</v>
@@ -7695,16 +7695,16 @@
         <v>295</v>
       </c>
       <c r="I58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J58">
-        <v>8.6393727974605264E-5</v>
+        <v>1.0051696893907487E-4</v>
       </c>
       <c r="M58" t="s">
         <v>14</v>
       </c>
       <c r="N58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -7727,19 +7727,19 @@
         <v>295</v>
       </c>
       <c r="I59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J59">
-        <v>0.17233571923239779</v>
+        <v>9.1258438035610265E-5</v>
       </c>
       <c r="M59" t="s">
         <v>14</v>
       </c>
       <c r="N59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O59">
-        <v>8.7116423410277699E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.45">
@@ -7759,19 +7759,19 @@
         <v>295</v>
       </c>
       <c r="I60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J60">
-        <v>8.502771822542983E-2</v>
+        <v>8.3508551676683408E-5</v>
       </c>
       <c r="M60" t="s">
         <v>14</v>
       </c>
       <c r="N60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O60">
-        <v>0.15925465090432156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.45">
@@ -7791,19 +7791,19 @@
         <v>295</v>
       </c>
       <c r="I61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J61">
-        <v>2.462240912782411E-2</v>
+        <v>0.16492398164264874</v>
       </c>
       <c r="M61" t="s">
         <v>14</v>
       </c>
       <c r="N61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O61">
-        <v>9.0958227951374759E-2</v>
+        <v>9.5265653495440583E-2</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.45">
@@ -7823,19 +7823,19 @@
         <v>295</v>
       </c>
       <c r="I62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J62">
-        <v>1.1991418548987395E-4</v>
+        <v>9.2208887285114241E-2</v>
       </c>
       <c r="M62" t="s">
         <v>14</v>
       </c>
       <c r="N62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O62">
-        <v>0</v>
+        <v>0.12076367435944024</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.45">
@@ -7855,19 +7855,19 @@
         <v>295</v>
       </c>
       <c r="I63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J63">
-        <v>1.1967900135873763E-4</v>
+        <v>2.5447133164488274E-2</v>
       </c>
       <c r="M63" t="s">
         <v>14</v>
       </c>
       <c r="N63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O63">
-        <v>0</v>
+        <v>7.2916205414199187E-2</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.45">
@@ -7887,16 +7887,16 @@
         <v>295</v>
       </c>
       <c r="I64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J64">
-        <v>1.2021351074768381E-4</v>
+        <v>1.165088956506691E-4</v>
       </c>
       <c r="M64" t="s">
         <v>14</v>
       </c>
       <c r="N64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O64">
         <v>0</v>
@@ -7919,16 +7919,16 @@
         <v>295</v>
       </c>
       <c r="I65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J65">
-        <v>1.2741869731067789E-4</v>
+        <v>1.1590957110557877E-4</v>
       </c>
       <c r="M65" t="s">
         <v>14</v>
       </c>
       <c r="N65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O65">
         <v>0</v>
@@ -7951,16 +7951,16 @@
         <v>295</v>
       </c>
       <c r="I66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J66">
-        <v>1.4253462283007502E-4</v>
+        <v>1.156822411057169E-4</v>
       </c>
       <c r="M66" t="s">
         <v>14</v>
       </c>
       <c r="N66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O66">
         <v>0</v>
@@ -7983,16 +7983,16 @@
         <v>295</v>
       </c>
       <c r="I67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J67">
-        <v>1.5583321642705526E-4</v>
+        <v>1.1619890019631204E-4</v>
       </c>
       <c r="M67" t="s">
         <v>14</v>
       </c>
       <c r="N67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O67">
         <v>0</v>
@@ -8015,16 +8015,16 @@
         <v>295</v>
       </c>
       <c r="I68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J68">
-        <v>1.6156315707655796E-4</v>
+        <v>1.2316346473753429E-4</v>
       </c>
       <c r="M68" t="s">
         <v>14</v>
       </c>
       <c r="N68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O68">
         <v>0</v>
@@ -8047,16 +8047,16 @@
         <v>295</v>
       </c>
       <c r="I69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J69">
-        <v>1.6211904684106196E-4</v>
+        <v>1.377745838195644E-4</v>
       </c>
       <c r="M69" t="s">
         <v>14</v>
       </c>
       <c r="N69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O69">
         <v>0</v>
@@ -8079,16 +8079,16 @@
         <v>295</v>
       </c>
       <c r="I70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J70">
-        <v>1.6288874036114444E-4</v>
+        <v>1.5062906199357108E-4</v>
       </c>
       <c r="M70" t="s">
         <v>14</v>
       </c>
       <c r="N70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O70">
         <v>0</v>
@@ -8111,16 +8111,16 @@
         <v>295</v>
       </c>
       <c r="I71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J71">
-        <v>1.6293150111226012E-4</v>
+        <v>1.5616764744475078E-4</v>
       </c>
       <c r="M71" t="s">
         <v>14</v>
       </c>
       <c r="N71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O71">
         <v>0</v>
@@ -8143,16 +8143,16 @@
         <v>295</v>
       </c>
       <c r="I72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J72">
-        <v>1.6293150111226012E-4</v>
+        <v>1.5670497289896972E-4</v>
       </c>
       <c r="M72" t="s">
         <v>14</v>
       </c>
       <c r="N72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O72">
         <v>0</v>
@@ -8175,16 +8175,16 @@
         <v>295</v>
       </c>
       <c r="I73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J73">
-        <v>1.624611328499875E-4</v>
+        <v>1.574489619894267E-4</v>
       </c>
       <c r="M73" t="s">
         <v>14</v>
       </c>
       <c r="N73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O73">
         <v>0</v>
@@ -8207,16 +8207,16 @@
         <v>295</v>
       </c>
       <c r="I74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J74">
-        <v>1.6229008984552473E-4</v>
+        <v>1.5749029471667431E-4</v>
       </c>
       <c r="M74" t="s">
         <v>14</v>
       </c>
       <c r="N74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O74">
         <v>0</v>
@@ -8239,16 +8239,16 @@
         <v>295</v>
       </c>
       <c r="I75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J75">
-        <v>1.6229008984552473E-4</v>
+        <v>1.5749029471667431E-4</v>
       </c>
       <c r="M75" t="s">
         <v>14</v>
       </c>
       <c r="N75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O75">
         <v>0</v>
@@ -8271,16 +8271,16 @@
         <v>295</v>
       </c>
       <c r="I76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J76">
-        <v>1.6320944599451212E-4</v>
+        <v>1.5703563471695061E-4</v>
       </c>
       <c r="M76" t="s">
         <v>14</v>
       </c>
       <c r="N76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O76">
         <v>0</v>
@@ -8303,16 +8303,16 @@
         <v>295</v>
       </c>
       <c r="I77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J77">
-        <v>1.6350877125232194E-4</v>
+        <v>1.5687030380796016E-4</v>
       </c>
       <c r="M77" t="s">
         <v>14</v>
       </c>
       <c r="N77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O77">
         <v>0</v>
@@ -8335,16 +8335,16 @@
         <v>295</v>
       </c>
       <c r="I78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J78">
-        <v>1.6415018251905733E-4</v>
+        <v>1.5687030380796016E-4</v>
       </c>
       <c r="M78" t="s">
         <v>14</v>
       </c>
       <c r="N78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O78">
         <v>0</v>
@@ -8367,16 +8367,16 @@
         <v>295</v>
       </c>
       <c r="I79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J79">
-        <v>1.630170226144915E-4</v>
+        <v>1.5775895744378376E-4</v>
       </c>
       <c r="M79" t="s">
         <v>14</v>
       </c>
       <c r="N79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O79">
         <v>0</v>
@@ -8399,16 +8399,16 @@
         <v>295</v>
       </c>
       <c r="I80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J80">
-        <v>1.5606840055819155E-4</v>
+        <v>1.5804828653451702E-4</v>
       </c>
       <c r="M80" t="s">
         <v>14</v>
       </c>
       <c r="N80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="O80">
         <v>0</v>
@@ -8431,16 +8431,16 @@
         <v>295</v>
       </c>
       <c r="I81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J81">
-        <v>1.3994759738757568E-4</v>
+        <v>1.5866827744323117E-4</v>
       </c>
       <c r="M81" t="s">
         <v>14</v>
       </c>
       <c r="N81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O81">
         <v>0</v>
@@ -8463,16 +8463,16 @@
         <v>295</v>
       </c>
       <c r="I82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J82">
-        <v>1.3075403589770187E-4</v>
+        <v>1.5757296017116954E-4</v>
       </c>
       <c r="M82" t="s">
         <v>14</v>
       </c>
       <c r="N82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O82">
         <v>0</v>
@@ -8495,16 +8495,16 @@
         <v>295</v>
       </c>
       <c r="I83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J83">
-        <v>1.227363950635096E-4</v>
+        <v>1.5085639199343293E-4</v>
       </c>
       <c r="M83" t="s">
         <v>14</v>
       </c>
       <c r="N83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O83">
         <v>0</v>
@@ -8527,16 +8527,16 @@
         <v>295</v>
       </c>
       <c r="I84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J84">
-        <v>1.2117562764778686E-4</v>
+        <v>1.3527395382108398E-4</v>
       </c>
       <c r="M84" t="s">
         <v>14</v>
       </c>
       <c r="N84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O84">
         <v>0</v>
@@ -8559,16 +8559,16 @@
         <v>295</v>
       </c>
       <c r="I85" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J85">
-        <v>1.1991418548987395E-4</v>
+        <v>1.2638741746284787E-4</v>
       </c>
       <c r="M85" t="s">
         <v>14</v>
       </c>
       <c r="N85" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="O85">
         <v>0</v>
@@ -8591,16 +8591,16 @@
         <v>295</v>
       </c>
       <c r="I86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J86">
-        <v>1.1967900135873763E-4</v>
+        <v>1.18637531103921E-4</v>
       </c>
       <c r="M86" t="s">
         <v>14</v>
       </c>
       <c r="N86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="O86">
         <v>0</v>
@@ -8623,16 +8623,16 @@
         <v>295</v>
       </c>
       <c r="I87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J87">
-        <v>1.199997069921053E-4</v>
+        <v>1.1712888655938323E-4</v>
       </c>
       <c r="M87" t="s">
         <v>14</v>
       </c>
       <c r="N87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O87">
         <v>0</v>
@@ -8655,16 +8655,16 @@
         <v>295</v>
       </c>
       <c r="I88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J88">
-        <v>1.2767526181737204E-4</v>
+        <v>1.165088956506691E-4</v>
       </c>
       <c r="M88" t="s">
         <v>14</v>
       </c>
       <c r="N88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="O88">
         <v>0</v>
@@ -8687,16 +8687,16 @@
         <v>295</v>
       </c>
       <c r="I89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J89">
-        <v>1.4279118733676917E-4</v>
+        <v>1.1590957110557877E-4</v>
       </c>
       <c r="M89" t="s">
         <v>14</v>
       </c>
       <c r="N89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O89">
         <v>0</v>
@@ -8719,16 +8719,16 @@
         <v>295</v>
       </c>
       <c r="I90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J90">
-        <v>1.554911304181297E-4</v>
+        <v>1.156822411057169E-4</v>
       </c>
       <c r="M90" t="s">
         <v>14</v>
       </c>
       <c r="N90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="O90">
         <v>0</v>
@@ -8751,16 +8751,16 @@
         <v>295</v>
       </c>
       <c r="I91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J91">
-        <v>1.6122107106763243E-4</v>
+        <v>1.1599223656007395E-4</v>
       </c>
       <c r="M91" t="s">
         <v>14</v>
       </c>
       <c r="N91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="O91">
         <v>0</v>
@@ -8783,16 +8783,16 @@
         <v>295</v>
       </c>
       <c r="I92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J92">
-        <v>1.6175558045657858E-4</v>
+        <v>1.2341146110101994E-4</v>
       </c>
       <c r="M92" t="s">
         <v>14</v>
       </c>
       <c r="N92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="O92">
         <v>0</v>
@@ -8815,16 +8815,16 @@
         <v>295</v>
       </c>
       <c r="I93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J93">
-        <v>1.6278183848335517E-4</v>
+        <v>1.3802258018305005E-4</v>
       </c>
       <c r="M93" t="s">
         <v>14</v>
       </c>
       <c r="N93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="O93">
         <v>0</v>
@@ -8847,16 +8847,16 @@
         <v>295</v>
       </c>
       <c r="I94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J94">
-        <v>1.624611328499875E-4</v>
+        <v>1.5029840017559016E-4</v>
       </c>
       <c r="M94" t="s">
         <v>14</v>
       </c>
       <c r="N94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="O94">
         <v>0</v>
@@ -8879,16 +8879,16 @@
         <v>295</v>
       </c>
       <c r="I95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J95">
-        <v>1.619480038365992E-4</v>
+        <v>1.5583698562676991E-4</v>
       </c>
       <c r="M95" t="s">
         <v>14</v>
       </c>
       <c r="N95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="O95">
         <v>0</v>
@@ -8911,16 +8911,16 @@
         <v>295</v>
       </c>
       <c r="I96" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J96">
-        <v>1.6124245144319028E-4</v>
+        <v>1.5635364471736505E-4</v>
       </c>
       <c r="M96" t="s">
         <v>14</v>
       </c>
       <c r="N96" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="O96">
         <v>0</v>
@@ -8943,16 +8943,16 @@
         <v>295</v>
       </c>
       <c r="I97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J97">
-        <v>1.6105002806316967E-4</v>
+        <v>1.5734563017130767E-4</v>
       </c>
       <c r="M97" t="s">
         <v>14</v>
       </c>
       <c r="N97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O97">
         <v>0</v>
@@ -8975,16 +8975,16 @@
         <v>295</v>
       </c>
       <c r="I98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J98">
-        <v>1.6105002806316967E-4</v>
+        <v>1.5703563471695058E-4</v>
       </c>
       <c r="M98" t="s">
         <v>14</v>
       </c>
       <c r="N98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O98">
         <v>0</v>
@@ -9007,16 +9007,16 @@
         <v>295</v>
       </c>
       <c r="I99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J99">
-        <v>1.6132797294542167E-4</v>
+        <v>1.5653964198997927E-4</v>
       </c>
       <c r="M99" t="s">
         <v>14</v>
       </c>
       <c r="N99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="O99">
         <v>0</v>
@@ -9039,16 +9039,16 @@
         <v>295</v>
       </c>
       <c r="I100" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J100">
-        <v>1.6222594871885117E-4</v>
+        <v>1.5585765199039372E-4</v>
       </c>
       <c r="M100" t="s">
         <v>14</v>
       </c>
       <c r="N100" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="O100">
         <v>0</v>
@@ -9071,16 +9071,16 @@
         <v>295</v>
       </c>
       <c r="I101" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J101">
-        <v>1.6350877125232194E-4</v>
+        <v>1.5567165471777947E-4</v>
       </c>
       <c r="M101" t="s">
         <v>14</v>
       </c>
       <c r="N101" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="O101">
         <v>0</v>
@@ -9103,16 +9103,16 @@
         <v>295</v>
       </c>
       <c r="I102" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J102">
-        <v>1.630170226144915E-4</v>
+        <v>1.5567165471777947E-4</v>
       </c>
       <c r="M102" t="s">
         <v>14</v>
       </c>
       <c r="N102" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="O102">
         <v>0</v>
@@ -9135,16 +9135,16 @@
         <v>295</v>
       </c>
       <c r="I103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J103">
-        <v>1.5606840055819153E-4</v>
+        <v>1.5594031744488895E-4</v>
       </c>
       <c r="M103" t="s">
         <v>14</v>
       </c>
       <c r="N103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="O103">
         <v>0</v>
@@ -9167,16 +9167,16 @@
         <v>295</v>
       </c>
       <c r="I104" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J104">
-        <v>1.3994759738757565E-4</v>
+        <v>1.5680830471708873E-4</v>
       </c>
       <c r="M104" t="s">
         <v>14</v>
       </c>
       <c r="N104" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O104">
         <v>0</v>
@@ -9199,16 +9199,16 @@
         <v>295</v>
       </c>
       <c r="I105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J105">
-        <v>1.3075403589770187E-4</v>
+        <v>1.5804828653451702E-4</v>
       </c>
       <c r="M105" t="s">
         <v>14</v>
       </c>
       <c r="N105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="O105">
         <v>0</v>
@@ -9231,16 +9231,16 @@
         <v>295</v>
       </c>
       <c r="I106" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J106">
-        <v>1.227363950635096E-4</v>
+        <v>1.5757296017116952E-4</v>
       </c>
       <c r="M106" t="s">
         <v>14</v>
       </c>
       <c r="N106" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="O106">
         <v>0</v>
@@ -9263,16 +9263,16 @@
         <v>295</v>
       </c>
       <c r="I107" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J107">
-        <v>1.2128252952557609E-4</v>
+        <v>1.5085639199343291E-4</v>
       </c>
       <c r="M107" t="s">
         <v>14</v>
       </c>
       <c r="N107" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="O107">
         <v>0</v>
@@ -9292,13 +9292,22 @@
         <v>291</v>
       </c>
       <c r="H108" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I108" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="J108">
-        <v>0.14340464718967832</v>
+        <v>1.3527395382108395E-4</v>
+      </c>
+      <c r="M108" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" t="s">
+        <v>284</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.45">
@@ -9315,13 +9324,22 @@
         <v>291</v>
       </c>
       <c r="H109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I109" t="s">
-        <v>181</v>
+        <v>285</v>
       </c>
       <c r="J109">
-        <v>8.6714808999295859E-2</v>
+        <v>1.2638741746284784E-4</v>
+      </c>
+      <c r="M109" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" t="s">
+        <v>285</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.45">
@@ -9338,13 +9356,22 @@
         <v>291</v>
       </c>
       <c r="H110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I110" t="s">
-        <v>182</v>
+        <v>286</v>
       </c>
       <c r="J110">
-        <v>2.1940825262755863E-2</v>
+        <v>1.18637531103921E-4</v>
+      </c>
+      <c r="M110" t="s">
+        <v>14</v>
+      </c>
+      <c r="N110" t="s">
+        <v>286</v>
+      </c>
+      <c r="O110">
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.45">
@@ -9361,13 +9388,22 @@
         <v>291</v>
       </c>
       <c r="H111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I111" t="s">
-        <v>183</v>
+        <v>287</v>
       </c>
       <c r="J111">
-        <v>0.14323738598044383</v>
+        <v>1.1723221837750227E-4</v>
+      </c>
+      <c r="M111" t="s">
+        <v>14</v>
+      </c>
+      <c r="N111" t="s">
+        <v>287</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.45">
@@ -9375,10 +9411,10 @@
         <v>296</v>
       </c>
       <c r="I112" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J112">
-        <v>8.6688081865098243E-2</v>
+        <v>0.13742785239842162</v>
       </c>
     </row>
     <row r="113" spans="8:10" x14ac:dyDescent="0.45">
@@ -9386,10 +9422,10 @@
         <v>296</v>
       </c>
       <c r="I113" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J113">
-        <v>2.1918598943937953E-2</v>
+        <v>9.3505477171915943E-2</v>
       </c>
     </row>
     <row r="114" spans="8:10" x14ac:dyDescent="0.45">
@@ -9397,10 +9433,10 @@
         <v>296</v>
       </c>
       <c r="I114" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J114">
-        <v>0.13866798023969606</v>
+        <v>2.111999417267961E-2</v>
       </c>
     </row>
     <row r="115" spans="8:10" x14ac:dyDescent="0.45">
@@ -9408,10 +9444,10 @@
         <v>296</v>
       </c>
       <c r="I115" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J115">
-        <v>8.3833277824534383E-2</v>
+        <v>0.13724408438121266</v>
       </c>
     </row>
     <row r="116" spans="8:10" x14ac:dyDescent="0.45">
@@ -9419,10 +9455,10 @@
         <v>296</v>
       </c>
       <c r="I116" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J116">
-        <v>2.1242776187173726E-2</v>
+        <v>9.3531718332046473E-2</v>
       </c>
     </row>
     <row r="117" spans="8:10" x14ac:dyDescent="0.45">
@@ -9430,10 +9466,10 @@
         <v>296</v>
       </c>
       <c r="I117" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J117">
-        <v>1.172860127846778E-4</v>
+        <v>2.1065816307503725E-2</v>
       </c>
     </row>
     <row r="118" spans="8:10" x14ac:dyDescent="0.45">
@@ -9441,10 +9477,10 @@
         <v>296</v>
       </c>
       <c r="I118" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J118">
-        <v>1.172995363049694E-4</v>
+        <v>0.13285026163930186</v>
       </c>
     </row>
     <row r="119" spans="8:10" x14ac:dyDescent="0.45">
@@ -9452,10 +9488,10 @@
         <v>296</v>
       </c>
       <c r="I119" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J119">
-        <v>1.1756399625733836E-4</v>
+        <v>9.0449861645704149E-2</v>
       </c>
     </row>
     <row r="120" spans="8:10" x14ac:dyDescent="0.45">
@@ -9463,10 +9499,10 @@
         <v>296</v>
       </c>
       <c r="I120" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J120">
-        <v>1.1810493706900214E-4</v>
+        <v>2.0437873349246113E-2</v>
       </c>
     </row>
     <row r="121" spans="8:10" x14ac:dyDescent="0.45">
@@ -9474,10 +9510,10 @@
         <v>296</v>
       </c>
       <c r="I121" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J121">
-        <v>1.1893137442015512E-4</v>
+        <v>1.1251571921392977E-4</v>
       </c>
     </row>
     <row r="122" spans="8:10" x14ac:dyDescent="0.45">
@@ -9485,10 +9521,10 @@
         <v>296</v>
       </c>
       <c r="I122" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J122">
-        <v>1.1983294243959474E-4</v>
+        <v>1.1246672960092364E-4</v>
       </c>
     </row>
     <row r="123" spans="8:10" x14ac:dyDescent="0.45">
@@ -9496,10 +9532,10 @@
         <v>296</v>
       </c>
       <c r="I123" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J123">
-        <v>1.2052113936110033E-4</v>
+        <v>1.1247969743966055E-4</v>
       </c>
     </row>
     <row r="124" spans="8:10" x14ac:dyDescent="0.45">
@@ -9507,10 +9543,10 @@
         <v>296</v>
       </c>
       <c r="I124" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J124">
-        <v>1.2073150523230291E-4</v>
+        <v>1.1273329073051577E-4</v>
       </c>
     </row>
     <row r="125" spans="8:10" x14ac:dyDescent="0.45">
@@ -9518,10 +9554,10 @@
         <v>296</v>
       </c>
       <c r="I125" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J125">
-        <v>1.2075254181942316E-4</v>
+        <v>1.1325200427999234E-4</v>
       </c>
     </row>
     <row r="126" spans="8:10" x14ac:dyDescent="0.45">
@@ -9529,10 +9565,10 @@
         <v>296</v>
       </c>
       <c r="I126" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J126">
-        <v>1.2075254181942316E-4</v>
+        <v>1.1404448331391486E-4</v>
       </c>
     </row>
     <row r="127" spans="8:10" x14ac:dyDescent="0.45">
@@ -9540,10 +9576,10 @@
         <v>296</v>
       </c>
       <c r="I127" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J127">
-        <v>1.2072098693874278E-4</v>
+        <v>1.1490900589637579E-4</v>
       </c>
     </row>
     <row r="128" spans="8:10" x14ac:dyDescent="0.45">
@@ -9551,10 +9587,10 @@
         <v>296</v>
       </c>
       <c r="I128" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J128">
-        <v>1.2072098693874278E-4</v>
+        <v>1.1556892480098766E-4</v>
       </c>
     </row>
     <row r="129" spans="8:10" x14ac:dyDescent="0.45">
@@ -9562,10 +9598,10 @@
         <v>296</v>
       </c>
       <c r="I129" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J129">
-        <v>1.2061880922987296E-4</v>
+        <v>1.1577064673689521E-4</v>
       </c>
     </row>
     <row r="130" spans="8:10" x14ac:dyDescent="0.45">
@@ -9573,10 +9609,10 @@
         <v>296</v>
       </c>
       <c r="I130" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J130">
-        <v>1.2060378309621561E-4</v>
+        <v>1.1579081893048595E-4</v>
       </c>
     </row>
     <row r="131" spans="8:10" x14ac:dyDescent="0.45">
@@ -9584,10 +9620,10 @@
         <v>296</v>
       </c>
       <c r="I131" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J131">
-        <v>1.205842491224611E-4</v>
+        <v>1.1579081893048595E-4</v>
       </c>
     </row>
     <row r="132" spans="8:10" x14ac:dyDescent="0.45">
@@ -9595,10 +9631,10 @@
         <v>296</v>
       </c>
       <c r="I132" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J132">
-        <v>1.2055870469524364E-4</v>
+        <v>1.1576056064009983E-4</v>
       </c>
     </row>
     <row r="133" spans="8:10" x14ac:dyDescent="0.45">
@@ -9606,10 +9642,10 @@
         <v>296</v>
       </c>
       <c r="I133" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J133">
-        <v>1.2048808186705421E-4</v>
+        <v>1.1576056064009983E-4</v>
       </c>
     </row>
     <row r="134" spans="8:10" x14ac:dyDescent="0.45">
@@ -9617,10 +9653,10 @@
         <v>296</v>
       </c>
       <c r="I134" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J134">
-        <v>1.2041595642549904E-4</v>
+        <v>1.1566258141408759E-4</v>
       </c>
     </row>
     <row r="135" spans="8:10" x14ac:dyDescent="0.45">
@@ -9628,10 +9664,10 @@
         <v>296</v>
       </c>
       <c r="I135" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J135">
-        <v>1.2016501999342167E-4</v>
+        <v>1.1564817270437989E-4</v>
       </c>
     </row>
     <row r="136" spans="8:10" x14ac:dyDescent="0.45">
@@ -9639,10 +9675,10 @@
         <v>296</v>
       </c>
       <c r="I136" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="J136">
-        <v>1.193581166160232E-4</v>
+        <v>1.1562944138175992E-4</v>
       </c>
     </row>
     <row r="137" spans="8:10" x14ac:dyDescent="0.45">
@@ -9650,10 +9686,10 @@
         <v>296</v>
       </c>
       <c r="I137" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J137">
-        <v>1.1888028556572021E-4</v>
+        <v>1.1560494657525684E-4</v>
       </c>
     </row>
     <row r="138" spans="8:10" x14ac:dyDescent="0.45">
@@ -9661,10 +9697,10 @@
         <v>296</v>
       </c>
       <c r="I138" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J138">
-        <v>1.1828374805952434E-4</v>
+        <v>1.1553722563963075E-4</v>
       </c>
     </row>
     <row r="139" spans="8:10" x14ac:dyDescent="0.45">
@@ -9672,10 +9708,10 @@
         <v>296</v>
       </c>
       <c r="I139" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J139">
-        <v>1.1769021578005991E-4</v>
+        <v>1.1546806383303387E-4</v>
       </c>
     </row>
     <row r="140" spans="8:10" x14ac:dyDescent="0.45">
@@ -9683,10 +9719,10 @@
         <v>296</v>
       </c>
       <c r="I140" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J140">
-        <v>1.1726046835746037E-4</v>
+        <v>1.1522743838091558E-4</v>
       </c>
     </row>
     <row r="141" spans="8:10" x14ac:dyDescent="0.45">
@@ -9694,10 +9730,10 @@
         <v>296</v>
       </c>
       <c r="I141" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J141">
-        <v>1.1732057289208968E-4</v>
+        <v>1.1445369066961302E-4</v>
       </c>
     </row>
     <row r="142" spans="8:10" x14ac:dyDescent="0.45">
@@ -9705,10 +9741,10 @@
         <v>296</v>
       </c>
       <c r="I142" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J142">
-        <v>1.1762560340533342E-4</v>
+        <v>1.1399549370090874E-4</v>
       </c>
     </row>
     <row r="143" spans="8:10" x14ac:dyDescent="0.45">
@@ -9716,10 +9752,10 @@
         <v>296</v>
       </c>
       <c r="I143" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J143">
-        <v>1.182506905654782E-4</v>
+        <v>1.1342346792551377E-4</v>
       </c>
     </row>
     <row r="144" spans="8:10" x14ac:dyDescent="0.45">
@@ -9727,10 +9763,10 @@
         <v>296</v>
       </c>
       <c r="I144" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J144">
-        <v>1.1905759394287667E-4</v>
+        <v>1.1285432389206029E-4</v>
       </c>
     </row>
     <row r="145" spans="8:10" x14ac:dyDescent="0.45">
@@ -9738,10 +9774,10 @@
         <v>296</v>
       </c>
       <c r="I145" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="J145">
-        <v>1.2008988932513504E-4</v>
+        <v>1.1247393395577749E-4</v>
       </c>
     </row>
     <row r="146" spans="8:10" x14ac:dyDescent="0.45">
@@ -9749,10 +9785,10 @@
         <v>296</v>
       </c>
       <c r="I146" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="J146">
-        <v>1.2075554704615462E-4</v>
+        <v>1.1244223479442061E-4</v>
       </c>
     </row>
     <row r="147" spans="8:10" x14ac:dyDescent="0.45">
@@ -9760,10 +9796,10 @@
         <v>296</v>
       </c>
       <c r="I147" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J147">
-        <v>1.2077508101990916E-4</v>
+        <v>1.1249986963325132E-4</v>
       </c>
     </row>
     <row r="148" spans="8:10" x14ac:dyDescent="0.45">
@@ -9771,10 +9807,10 @@
         <v>296</v>
       </c>
       <c r="I148" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J148">
-        <v>1.2073751568576584E-4</v>
+        <v>1.1279236644031727E-4</v>
       </c>
     </row>
     <row r="149" spans="8:10" x14ac:dyDescent="0.45">
@@ -9782,10 +9818,10 @@
         <v>296</v>
       </c>
       <c r="I149" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J149">
-        <v>1.207269973922057E-4</v>
+        <v>1.1339176876415685E-4</v>
       </c>
     </row>
     <row r="150" spans="8:10" x14ac:dyDescent="0.45">
@@ -9793,10 +9829,10 @@
         <v>296</v>
       </c>
       <c r="I150" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="J150">
-        <v>1.207360130724001E-4</v>
+        <v>1.1416551647545939E-4</v>
       </c>
     </row>
     <row r="151" spans="8:10" x14ac:dyDescent="0.45">
@@ -9804,10 +9840,10 @@
         <v>296</v>
       </c>
       <c r="I151" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J151">
-        <v>1.2074803397932596E-4</v>
+        <v>1.1515539483237717E-4</v>
       </c>
     </row>
     <row r="152" spans="8:10" x14ac:dyDescent="0.45">
@@ -9815,10 +9851,10 @@
         <v>296</v>
       </c>
       <c r="I152" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J152">
-        <v>1.2067891376450227E-4</v>
+        <v>1.1579370067242749E-4</v>
       </c>
     </row>
     <row r="153" spans="8:10" x14ac:dyDescent="0.45">
@@ -9826,10 +9862,10 @@
         <v>296</v>
       </c>
       <c r="I153" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J153">
-        <v>1.2065937979074774E-4</v>
+        <v>1.1581243199504749E-4</v>
       </c>
     </row>
     <row r="154" spans="8:10" x14ac:dyDescent="0.45">
@@ -9837,10 +9873,10 @@
         <v>296</v>
       </c>
       <c r="I154" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J154">
-        <v>1.2063984581699321E-4</v>
+        <v>1.1577641022077827E-4</v>
       </c>
     </row>
     <row r="155" spans="8:10" x14ac:dyDescent="0.45">
@@ -9848,10 +9884,10 @@
         <v>296</v>
       </c>
       <c r="I155" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J155">
-        <v>1.2061430138977575E-4</v>
+        <v>1.1576632412398289E-4</v>
       </c>
     </row>
     <row r="156" spans="8:10" x14ac:dyDescent="0.45">
@@ -9859,10 +9895,10 @@
         <v>296</v>
       </c>
       <c r="I156" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J156">
-        <v>1.2056020730860936E-4</v>
+        <v>1.157749693498075E-4</v>
       </c>
     </row>
     <row r="157" spans="8:10" x14ac:dyDescent="0.45">
@@ -9870,10 +9906,10 @@
         <v>296</v>
       </c>
       <c r="I157" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="J157">
-        <v>1.2047155312003115E-4</v>
+        <v>1.1578649631757366E-4</v>
       </c>
     </row>
     <row r="158" spans="8:10" x14ac:dyDescent="0.45">
@@ -9881,10 +9917,10 @@
         <v>296</v>
       </c>
       <c r="I158" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J158">
-        <v>1.2020258532756499E-4</v>
+        <v>1.1572021625291832E-4</v>
       </c>
     </row>
     <row r="159" spans="8:10" x14ac:dyDescent="0.45">
@@ -9892,10 +9928,10 @@
         <v>296</v>
       </c>
       <c r="I159" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J159">
-        <v>1.193806558165092E-4</v>
+        <v>1.1570148493029833E-4</v>
       </c>
     </row>
     <row r="160" spans="8:10" x14ac:dyDescent="0.45">
@@ -9903,10 +9939,10 @@
         <v>296</v>
       </c>
       <c r="I160" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J160">
-        <v>1.1894489794044672E-4</v>
+        <v>1.1568275360767833E-4</v>
       </c>
     </row>
     <row r="161" spans="8:10" x14ac:dyDescent="0.45">
@@ -9914,10 +9950,10 @@
         <v>296</v>
       </c>
       <c r="I161" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="J161">
-        <v>1.1827172715259848E-4</v>
+        <v>1.1565825880117527E-4</v>
       </c>
     </row>
     <row r="162" spans="8:10" x14ac:dyDescent="0.45">
@@ -9925,10 +9961,10 @@
         <v>296</v>
       </c>
       <c r="I162" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J162">
-        <v>1.1770824714044871E-4</v>
+        <v>1.1560638744622761E-4</v>
       </c>
     </row>
     <row r="163" spans="8:10" x14ac:dyDescent="0.45">
@@ -9936,10 +9972,10 @@
         <v>296</v>
       </c>
       <c r="I163" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="J163">
-        <v>0.13732012449245445</v>
+        <v>1.155213760589523E-4</v>
       </c>
     </row>
     <row r="164" spans="8:10" x14ac:dyDescent="0.45">
@@ -9947,10 +9983,10 @@
         <v>296</v>
       </c>
       <c r="I164" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J164">
-        <v>8.3027052179348013E-2</v>
+        <v>1.1526346015518479E-4</v>
       </c>
     </row>
     <row r="165" spans="8:10" x14ac:dyDescent="0.45">
@@ -9958,10 +9994,10 @@
         <v>296</v>
       </c>
       <c r="I165" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J165">
-        <v>2.0993289039083644E-2</v>
+        <v>1.1447530373417456E-4</v>
       </c>
     </row>
     <row r="166" spans="8:10" x14ac:dyDescent="0.45">
@@ -9969,10 +10005,10 @@
         <v>296</v>
       </c>
       <c r="I166" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J166">
-        <v>1.1776438901703989E-4</v>
+        <v>1.1405745115265177E-4</v>
       </c>
     </row>
     <row r="167" spans="8:10" x14ac:dyDescent="0.45">
@@ -9980,10 +10016,10 @@
         <v>296</v>
       </c>
       <c r="I167" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J167">
-        <v>1.1774786027001683E-4</v>
+        <v>1.1341194095774761E-4</v>
       </c>
     </row>
     <row r="168" spans="8:10" x14ac:dyDescent="0.45">
@@ -9991,10 +10027,10 @@
         <v>296</v>
       </c>
       <c r="I168" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J168">
-        <v>1.1778542560416013E-4</v>
+        <v>1.1287161434370953E-4</v>
       </c>
     </row>
     <row r="169" spans="8:10" x14ac:dyDescent="0.45">
@@ -10002,10 +10038,10 @@
         <v>296</v>
       </c>
       <c r="I169" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="J169">
-        <v>1.1829180630841204E-4</v>
+        <v>0.13156214937082664</v>
       </c>
     </row>
     <row r="170" spans="8:10" x14ac:dyDescent="0.45">
@@ -10013,10 +10049,10 @@
         <v>296</v>
       </c>
       <c r="I170" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J170">
-        <v>1.1935415395798507E-4</v>
+        <v>8.9549778785707551E-2</v>
       </c>
     </row>
     <row r="171" spans="8:10" x14ac:dyDescent="0.45">
@@ -10024,10 +10060,10 @@
         <v>296</v>
       </c>
       <c r="I171" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J171">
-        <v>1.2028877947147082E-4</v>
+        <v>2.0245504840090894E-2</v>
       </c>
     </row>
     <row r="172" spans="8:10" x14ac:dyDescent="0.45">
@@ -10035,10 +10071,10 @@
         <v>296</v>
       </c>
       <c r="I172" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="J172">
-        <v>1.2069147985348719E-4</v>
+        <v>1.1296723460830421E-4</v>
       </c>
     </row>
     <row r="173" spans="8:10" x14ac:dyDescent="0.45">
@@ -10046,10 +10082,10 @@
         <v>296</v>
       </c>
       <c r="I173" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J173">
-        <v>1.2073054780099625E-4</v>
+        <v>1.1292544935015194E-4</v>
       </c>
     </row>
     <row r="174" spans="8:10" x14ac:dyDescent="0.45">
@@ -10057,10 +10093,10 @@
         <v>296</v>
       </c>
       <c r="I174" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J174">
-        <v>1.2078464188216262E-4</v>
+        <v>1.1290959976947349E-4</v>
       </c>
     </row>
     <row r="175" spans="8:10" x14ac:dyDescent="0.45">
@@ -10068,10 +10104,10 @@
         <v>296</v>
       </c>
       <c r="I175" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J175">
-        <v>1.2078764710889408E-4</v>
+        <v>1.1294562154374269E-4</v>
       </c>
     </row>
     <row r="176" spans="8:10" x14ac:dyDescent="0.45">
@@ -10079,10 +10115,10 @@
         <v>296</v>
       </c>
       <c r="I176" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J176">
-        <v>1.2078764710889408E-4</v>
+        <v>1.1343119506089157E-4</v>
       </c>
     </row>
     <row r="177" spans="8:10" x14ac:dyDescent="0.45">
@@ -10090,10 +10126,10 @@
         <v>296</v>
       </c>
       <c r="I177" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="J177">
-        <v>1.2075458961484794E-4</v>
+        <v>1.1444989083722471E-4</v>
       </c>
     </row>
     <row r="178" spans="8:10" x14ac:dyDescent="0.45">
@@ -10101,10 +10137,10 @@
         <v>296</v>
       </c>
       <c r="I178" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J178">
-        <v>1.2074256870792211E-4</v>
+        <v>1.1534611258104255E-4</v>
       </c>
     </row>
     <row r="179" spans="8:10" x14ac:dyDescent="0.45">
@@ -10112,10 +10148,10 @@
         <v>296</v>
       </c>
       <c r="I179" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="J179">
-        <v>1.2074256870792211E-4</v>
+        <v>1.1573226600120844E-4</v>
       </c>
     </row>
     <row r="180" spans="8:10" x14ac:dyDescent="0.45">
@@ -10123,10 +10159,10 @@
         <v>296</v>
       </c>
       <c r="I180" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="J180">
-        <v>1.208071810826486E-4</v>
+        <v>1.1576972864644843E-4</v>
       </c>
     </row>
     <row r="181" spans="8:10" x14ac:dyDescent="0.45">
@@ -10134,10 +10170,10 @@
         <v>296</v>
       </c>
       <c r="I181" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="J181">
-        <v>1.2082821766976886E-4</v>
+        <v>1.1582160000139609E-4</v>
       </c>
     </row>
     <row r="182" spans="8:10" x14ac:dyDescent="0.45">
@@ -10145,10 +10181,10 @@
         <v>296</v>
       </c>
       <c r="I182" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="J182">
-        <v>1.2087329607074085E-4</v>
+        <v>1.1582448174333761E-4</v>
       </c>
     </row>
     <row r="183" spans="8:10" x14ac:dyDescent="0.45">
@@ -10156,10 +10192,10 @@
         <v>296</v>
       </c>
       <c r="I183" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="J183">
-        <v>1.20793657562357E-4</v>
+        <v>1.1582448174333761E-4</v>
       </c>
     </row>
     <row r="184" spans="8:10" x14ac:dyDescent="0.45">
@@ -10167,10 +10203,10 @@
         <v>296</v>
       </c>
       <c r="I184" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J184">
-        <v>1.2030530821849387E-4</v>
+        <v>1.157927825819807E-4</v>
       </c>
     </row>
     <row r="185" spans="8:10" x14ac:dyDescent="0.45">
@@ -10178,10 +10214,10 @@
         <v>296</v>
       </c>
       <c r="I185" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J185">
-        <v>1.1917233774073141E-4</v>
+        <v>1.1578125561421458E-4</v>
       </c>
     </row>
     <row r="186" spans="8:10" x14ac:dyDescent="0.45">
@@ -10189,10 +10225,10 @@
         <v>296</v>
       </c>
       <c r="I186" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J186">
-        <v>1.1852621399346635E-4</v>
+        <v>1.1578125561421458E-4</v>
       </c>
     </row>
     <row r="187" spans="8:10" x14ac:dyDescent="0.45">
@@ -10200,10 +10236,10 @@
         <v>296</v>
       </c>
       <c r="I187" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J187">
-        <v>1.179627339813166E-4</v>
+        <v>1.158432130659576E-4</v>
       </c>
     </row>
     <row r="188" spans="8:10" x14ac:dyDescent="0.45">
@@ -10211,10 +10247,10 @@
         <v>296</v>
       </c>
       <c r="I188" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J188">
-        <v>1.178530432056181E-4</v>
+        <v>1.1586338525954836E-4</v>
       </c>
     </row>
     <row r="189" spans="8:10" x14ac:dyDescent="0.45">
@@ -10222,10 +10258,10 @@
         <v>296</v>
       </c>
       <c r="I189" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J189">
-        <v>1.1776438901703989E-4</v>
+        <v>1.159066113886714E-4</v>
       </c>
     </row>
     <row r="190" spans="8:10" x14ac:dyDescent="0.45">
@@ -10233,10 +10269,10 @@
         <v>296</v>
       </c>
       <c r="I190" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="J190">
-        <v>1.1774786027001683E-4</v>
+        <v>1.1583024522722069E-4</v>
       </c>
     </row>
     <row r="191" spans="8:10" x14ac:dyDescent="0.45">
@@ -10244,10 +10280,10 @@
         <v>296</v>
       </c>
       <c r="I191" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J191">
-        <v>1.1777039947050282E-4</v>
+        <v>1.1536196216172101E-4</v>
       </c>
     </row>
     <row r="192" spans="8:10" x14ac:dyDescent="0.45">
@@ -10255,10 +10291,10 @@
         <v>296</v>
       </c>
       <c r="I192" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="J192">
-        <v>1.1830983766880086E-4</v>
+        <v>1.1427554544976176E-4</v>
       </c>
     </row>
     <row r="193" spans="8:10" x14ac:dyDescent="0.45">
@@ -10266,10 +10302,10 @@
         <v>296</v>
       </c>
       <c r="I193" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="J193">
-        <v>1.1937218531837388E-4</v>
+        <v>1.1365597093233142E-4</v>
       </c>
     </row>
     <row r="194" spans="8:10" x14ac:dyDescent="0.45">
@@ -10277,10 +10313,10 @@
         <v>296</v>
       </c>
       <c r="I194" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="J194">
-        <v>1.2026473765761911E-4</v>
+        <v>1.1311564431829334E-4</v>
       </c>
     </row>
     <row r="195" spans="8:10" x14ac:dyDescent="0.45">
@@ -10288,10 +10324,10 @@
         <v>296</v>
       </c>
       <c r="I195" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J195">
-        <v>1.2066743803963548E-4</v>
+        <v>1.1301046073742726E-4</v>
       </c>
     </row>
     <row r="196" spans="8:10" x14ac:dyDescent="0.45">
@@ -10299,10 +10335,10 @@
         <v>296</v>
       </c>
       <c r="I196" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="J196">
-        <v>1.2070500337377879E-4</v>
+        <v>1.1296723460830421E-4</v>
       </c>
     </row>
     <row r="197" spans="8:10" x14ac:dyDescent="0.45">
@@ -10310,10 +10346,10 @@
         <v>296</v>
       </c>
       <c r="I197" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="J197">
-        <v>1.2077712881533397E-4</v>
+        <v>1.1292544935015194E-4</v>
       </c>
     </row>
     <row r="198" spans="8:10" x14ac:dyDescent="0.45">
@@ -10321,10 +10357,10 @@
         <v>296</v>
       </c>
       <c r="I198" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J198">
-        <v>1.2075458961484797E-4</v>
+        <v>1.1290959976947349E-4</v>
       </c>
     </row>
     <row r="199" spans="8:10" x14ac:dyDescent="0.45">
@@ -10332,10 +10368,10 @@
         <v>296</v>
       </c>
       <c r="I199" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="J199">
-        <v>1.2071852689407037E-4</v>
+        <v>1.1293121283403503E-4</v>
       </c>
     </row>
     <row r="200" spans="8:10" x14ac:dyDescent="0.45">
@@ -10343,10 +10379,10 @@
         <v>296</v>
       </c>
       <c r="I200" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J200">
-        <v>1.206689406530012E-4</v>
+        <v>1.134484855125408E-4</v>
       </c>
     </row>
     <row r="201" spans="8:10" x14ac:dyDescent="0.45">
@@ -10354,10 +10390,10 @@
         <v>296</v>
       </c>
       <c r="I201" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="J201">
-        <v>1.2065541713270962E-4</v>
+        <v>1.1446718128887394E-4</v>
       </c>
     </row>
     <row r="202" spans="8:10" x14ac:dyDescent="0.45">
@@ -10365,10 +10401,10 @@
         <v>296</v>
       </c>
       <c r="I202" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="J202">
-        <v>1.2065541713270962E-4</v>
+        <v>1.1532305864551028E-4</v>
       </c>
     </row>
     <row r="203" spans="8:10" x14ac:dyDescent="0.45">
@@ -10376,10 +10412,10 @@
         <v>296</v>
       </c>
       <c r="I203" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="J203">
-        <v>1.2067495110646413E-4</v>
+        <v>1.1570921206567616E-4</v>
       </c>
     </row>
     <row r="204" spans="8:10" x14ac:dyDescent="0.45">
@@ -10387,10 +10423,10 @@
         <v>296</v>
       </c>
       <c r="I204" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="J204">
-        <v>1.2073806086782491E-4</v>
+        <v>1.1574523383994536E-4</v>
       </c>
     </row>
     <row r="205" spans="8:10" x14ac:dyDescent="0.45">
@@ -10398,10 +10434,10 @@
         <v>296</v>
       </c>
       <c r="I205" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="J205">
-        <v>1.2082821766976886E-4</v>
+        <v>1.1581439564654225E-4</v>
       </c>
     </row>
     <row r="206" spans="8:10" x14ac:dyDescent="0.45">
@@ -10409,10 +10445,10 @@
         <v>296</v>
       </c>
       <c r="I206" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="J206">
-        <v>1.2079365756235703E-4</v>
+        <v>1.1579278258198072E-4</v>
       </c>
     </row>
     <row r="207" spans="8:10" x14ac:dyDescent="0.45">
@@ -10420,10 +10456,10 @@
         <v>296</v>
       </c>
       <c r="I207" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="J207">
-        <v>1.2030530821849389E-4</v>
+        <v>1.1575820167868227E-4</v>
       </c>
     </row>
     <row r="208" spans="8:10" x14ac:dyDescent="0.45">
@@ -10431,10 +10467,10 @@
         <v>296</v>
       </c>
       <c r="I208" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="J208">
-        <v>1.1917233774073144E-4</v>
+        <v>1.1571065293664693E-4</v>
       </c>
     </row>
     <row r="209" spans="8:10" x14ac:dyDescent="0.45">
@@ -10442,10 +10478,10 @@
         <v>296</v>
       </c>
       <c r="I209" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J209">
-        <v>1.1852621399346638E-4</v>
+        <v>1.1569768509791002E-4</v>
       </c>
     </row>
     <row r="210" spans="8:10" x14ac:dyDescent="0.45">
@@ -10453,10 +10489,10 @@
         <v>296</v>
       </c>
       <c r="I210" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="J210">
-        <v>1.179627339813166E-4</v>
+        <v>1.1569768509791002E-4</v>
       </c>
     </row>
     <row r="211" spans="8:10" x14ac:dyDescent="0.45">
@@ -10464,10 +10500,98 @@
         <v>296</v>
       </c>
       <c r="I211" t="s">
+        <v>279</v>
+      </c>
+      <c r="J211">
+        <v>1.1571641642053E-4</v>
+      </c>
+    </row>
+    <row r="212" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H212" t="s">
+        <v>296</v>
+      </c>
+      <c r="I212" t="s">
+        <v>280</v>
+      </c>
+      <c r="J212">
+        <v>1.1577693300130227E-4</v>
+      </c>
+    </row>
+    <row r="213" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H213" t="s">
+        <v>296</v>
+      </c>
+      <c r="I213" t="s">
+        <v>281</v>
+      </c>
+      <c r="J213">
+        <v>1.1586338525954836E-4</v>
+      </c>
+    </row>
+    <row r="214" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H214" t="s">
+        <v>296</v>
+      </c>
+      <c r="I214" t="s">
+        <v>282</v>
+      </c>
+      <c r="J214">
+        <v>1.158302452272207E-4</v>
+      </c>
+    </row>
+    <row r="215" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H215" t="s">
+        <v>296</v>
+      </c>
+      <c r="I215" t="s">
+        <v>283</v>
+      </c>
+      <c r="J215">
+        <v>1.1536196216172102E-4</v>
+      </c>
+    </row>
+    <row r="216" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H216" t="s">
+        <v>296</v>
+      </c>
+      <c r="I216" t="s">
+        <v>284</v>
+      </c>
+      <c r="J216">
+        <v>1.1427554544976177E-4</v>
+      </c>
+    </row>
+    <row r="217" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H217" t="s">
+        <v>296</v>
+      </c>
+      <c r="I217" t="s">
+        <v>285</v>
+      </c>
+      <c r="J217">
+        <v>1.1365597093233144E-4</v>
+      </c>
+    </row>
+    <row r="218" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H218" t="s">
+        <v>296</v>
+      </c>
+      <c r="I218" t="s">
         <v>286</v>
       </c>
-      <c r="J211">
-        <v>1.1786055627244678E-4</v>
+      <c r="J218">
+        <v>1.1311564431829334E-4</v>
+      </c>
+    </row>
+    <row r="219" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H219" t="s">
+        <v>296</v>
+      </c>
+      <c r="I219" t="s">
+        <v>287</v>
+      </c>
+      <c r="J219">
+        <v>1.1301766509228111E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>